<commit_message>
feat: Phase 5 models & RDFs (those that we can push)
</commit_message>
<xml_diff>
--- a/Phase 3 - Language Definition/KGE24-UNITN - Language resource.xlsx
+++ b/Phase 3 - Language Definition/KGE24-UNITN - Language resource.xlsx
@@ -59,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="719">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="743" uniqueCount="726">
   <si>
     <t>ConcetID</t>
   </si>
@@ -610,7 +610,7 @@
     <t>KGE24-0A-34</t>
   </si>
   <si>
-    <t>served_days_sunay</t>
+    <t>served_days_sunday</t>
   </si>
   <si>
     <t>The considered servide is being provided each week on sunday</t>
@@ -727,6 +727,12 @@
     <t>identificatore unico per la risorsa OSM per un punto sulla mappa</t>
   </si>
   <si>
+    <t>KGE24-0A-49</t>
+  </si>
+  <si>
+    <t>stop_order</t>
+  </si>
+  <si>
     <t>Object Properties</t>
   </si>
   <si>
@@ -817,7 +823,7 @@
     <t xml:space="preserve">UKC-102589 </t>
   </si>
   <si>
-    <t>get off</t>
+    <t>get_off</t>
   </si>
   <si>
     <t>leave a vehicle, aircraft, etc.</t>
@@ -844,10 +850,10 @@
     <t>l'azione di salire a bordo di treni, autobus, navi, aereoplani, etc...</t>
   </si>
   <si>
-    <t>MISSING</t>
-  </si>
-  <si>
-    <t>using, travel by</t>
+    <t>KGE-0A-50</t>
+  </si>
+  <si>
+    <t>using, travel_by</t>
   </si>
   <si>
     <t>use a certain mean of transportation to travel</t>
@@ -887,6 +893,21 @@
   </si>
   <si>
     <t>svolgere compiti o ricoprire incarichi; servire in una funzione specifica</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UKC-106969 </t>
+  </si>
+  <si>
+    <t>inside</t>
+  </si>
+  <si>
+    <t>within a building</t>
+  </si>
+  <si>
+    <t>dentro</t>
+  </si>
+  <si>
+    <t>all'interno di un edificio</t>
   </si>
   <si>
     <t>Data Values</t>
@@ -3636,7 +3657,7 @@
         <v>63</v>
       </c>
       <c r="C19" s="35" t="str">
-        <f t="shared" ref="C19:C51" si="3">B19&amp;"_"&amp;A19</f>
+        <f t="shared" ref="C19:C52" si="3">B19&amp;"_"&amp;A19</f>
         <v>duration_UKC-72859</v>
       </c>
       <c r="D19" s="35" t="str">
@@ -4787,11 +4808,11 @@
       </c>
       <c r="C44" s="35" t="str">
         <f t="shared" si="3"/>
-        <v>served_days_sunay_KGE24-0A-34</v>
+        <v>served_days_sunday_KGE24-0A-34</v>
       </c>
       <c r="D44" s="35" t="str">
         <f t="shared" si="4"/>
-        <v>served_days_sunay_KGE24-0A-34</v>
+        <v>served_days_sunday_KGE24-0A-34</v>
       </c>
       <c r="E44" s="36" t="s">
         <v>184</v>
@@ -5147,12 +5168,19 @@
       <c r="AB51" s="4"/>
     </row>
     <row r="52" ht="17.25" customHeight="1">
-      <c r="A52" s="53"/>
-      <c r="B52" s="36"/>
-      <c r="C52" s="35"/>
+      <c r="A52" s="50" t="s">
+        <v>222</v>
+      </c>
+      <c r="B52" s="36" t="s">
+        <v>223</v>
+      </c>
+      <c r="C52" s="52" t="str">
+        <f t="shared" si="3"/>
+        <v>stop_order_KGE24-0A-49</v>
+      </c>
       <c r="D52" s="35" t="str">
         <f t="shared" si="4"/>
-        <v/>
+        <v>stop_order_KGE24-0A-49</v>
       </c>
       <c r="E52" s="49"/>
       <c r="F52" s="49"/>
@@ -5247,7 +5275,7 @@
     </row>
     <row r="55" ht="15.75" customHeight="1">
       <c r="A55" s="54" t="s">
-        <v>222</v>
+        <v>224</v>
       </c>
       <c r="B55" s="6"/>
       <c r="C55" s="6"/>
@@ -5279,13 +5307,13 @@
     </row>
     <row r="56" ht="15.75" customHeight="1">
       <c r="A56" s="55" t="s">
-        <v>223</v>
+        <v>225</v>
       </c>
       <c r="B56" s="56" t="s">
-        <v>224</v>
+        <v>226</v>
       </c>
       <c r="C56" s="57" t="str">
-        <f t="shared" ref="C56:C66" si="5">B56&amp;"_"&amp;A56</f>
+        <f t="shared" ref="C56:C67" si="5">B56&amp;"_"&amp;A56</f>
         <v>particpate_in, participate_UKC-97811</v>
       </c>
       <c r="D56" s="57" t="str">
@@ -5293,13 +5321,13 @@
         <v>particpate_in, participate_GID-97811</v>
       </c>
       <c r="E56" s="56" t="s">
-        <v>225</v>
+        <v>227</v>
       </c>
       <c r="F56" s="56" t="s">
-        <v>226</v>
+        <v>228</v>
       </c>
       <c r="G56" s="56" t="s">
-        <v>227</v>
+        <v>229</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4"/>
@@ -5325,10 +5353,10 @@
     </row>
     <row r="57" ht="15.75" customHeight="1">
       <c r="A57" s="55" t="s">
-        <v>228</v>
+        <v>230</v>
       </c>
       <c r="B57" s="56" t="s">
-        <v>229</v>
+        <v>231</v>
       </c>
       <c r="C57" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5339,13 +5367,13 @@
         <v>feel_GID-101373</v>
       </c>
       <c r="E57" s="56" t="s">
-        <v>230</v>
+        <v>232</v>
       </c>
       <c r="F57" s="56" t="s">
-        <v>231</v>
+        <v>233</v>
       </c>
       <c r="G57" s="56" t="s">
-        <v>232</v>
+        <v>234</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4"/>
@@ -5371,10 +5399,10 @@
     </row>
     <row r="58" ht="15.75" customHeight="1">
       <c r="A58" s="55" t="s">
-        <v>233</v>
+        <v>235</v>
       </c>
       <c r="B58" s="56" t="s">
-        <v>234</v>
+        <v>236</v>
       </c>
       <c r="C58" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5385,7 +5413,7 @@
         <v>is_a_GID-105454</v>
       </c>
       <c r="E58" s="56" t="s">
-        <v>235</v>
+        <v>237</v>
       </c>
       <c r="F58" s="58"/>
       <c r="G58" s="58"/>
@@ -5413,10 +5441,10 @@
     </row>
     <row r="59" ht="15.75" customHeight="1">
       <c r="A59" s="55" t="s">
-        <v>236</v>
+        <v>238</v>
       </c>
       <c r="B59" s="56" t="s">
-        <v>237</v>
+        <v>239</v>
       </c>
       <c r="C59" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5427,13 +5455,13 @@
         <v>located_GID-85982</v>
       </c>
       <c r="E59" s="56" t="s">
-        <v>238</v>
+        <v>240</v>
       </c>
       <c r="F59" s="56" t="s">
-        <v>239</v>
+        <v>241</v>
       </c>
       <c r="G59" s="56" t="s">
-        <v>240</v>
+        <v>242</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4"/>
@@ -5459,10 +5487,10 @@
     </row>
     <row r="60" ht="15.75" customHeight="1">
       <c r="A60" s="55" t="s">
-        <v>241</v>
+        <v>243</v>
       </c>
       <c r="B60" s="56" t="s">
-        <v>242</v>
+        <v>244</v>
       </c>
       <c r="C60" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5473,13 +5501,13 @@
         <v>stay_put_GID-101763</v>
       </c>
       <c r="E60" s="56" t="s">
-        <v>243</v>
+        <v>245</v>
       </c>
       <c r="F60" s="56" t="s">
-        <v>244</v>
+        <v>246</v>
       </c>
       <c r="G60" s="56" t="s">
-        <v>245</v>
+        <v>247</v>
       </c>
       <c r="H60" s="4"/>
       <c r="I60" s="4"/>
@@ -5505,10 +5533,10 @@
     </row>
     <row r="61" ht="15.75" customHeight="1">
       <c r="A61" s="55" t="s">
-        <v>246</v>
+        <v>248</v>
       </c>
       <c r="B61" s="56" t="s">
-        <v>247</v>
+        <v>249</v>
       </c>
       <c r="C61" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5519,13 +5547,13 @@
         <v>take_GID-101699 </v>
       </c>
       <c r="E61" s="56" t="s">
-        <v>248</v>
+        <v>250</v>
       </c>
       <c r="F61" s="56" t="s">
-        <v>249</v>
+        <v>251</v>
       </c>
       <c r="G61" s="56" t="s">
-        <v>250</v>
+        <v>252</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4"/>
@@ -5551,27 +5579,27 @@
     </row>
     <row r="62" ht="30.75" customHeight="1">
       <c r="A62" s="59" t="s">
-        <v>251</v>
+        <v>253</v>
       </c>
       <c r="B62" s="60" t="s">
-        <v>252</v>
+        <v>254</v>
       </c>
       <c r="C62" s="57" t="str">
         <f t="shared" si="5"/>
-        <v>get off_UKC-102589 </v>
+        <v>get_off_UKC-102589 </v>
       </c>
       <c r="D62" s="57" t="str">
         <f t="shared" si="6"/>
-        <v>get off_GID-102589 </v>
+        <v>get_off_GID-102589 </v>
       </c>
       <c r="E62" s="60" t="s">
-        <v>253</v>
+        <v>255</v>
       </c>
       <c r="F62" s="60" t="s">
-        <v>254</v>
+        <v>256</v>
       </c>
       <c r="G62" s="61" t="s">
-        <v>255</v>
+        <v>257</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="62"/>
@@ -5597,10 +5625,10 @@
     </row>
     <row r="63" ht="15.75" customHeight="1">
       <c r="A63" s="63" t="s">
-        <v>256</v>
+        <v>258</v>
       </c>
       <c r="B63" s="64" t="s">
-        <v>257</v>
+        <v>259</v>
       </c>
       <c r="C63" s="65" t="str">
         <f t="shared" si="5"/>
@@ -5611,13 +5639,13 @@
         <v>board_GID-102601</v>
       </c>
       <c r="E63" s="64" t="s">
-        <v>258</v>
+        <v>260</v>
       </c>
       <c r="F63" s="64" t="s">
-        <v>259</v>
+        <v>261</v>
       </c>
       <c r="G63" s="64" t="s">
-        <v>260</v>
+        <v>262</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4"/>
@@ -5643,27 +5671,27 @@
     </row>
     <row r="64" ht="15.75" customHeight="1">
       <c r="A64" s="63" t="s">
-        <v>261</v>
+        <v>263</v>
       </c>
       <c r="B64" s="64" t="s">
-        <v>262</v>
+        <v>264</v>
       </c>
       <c r="C64" s="65" t="str">
         <f t="shared" si="5"/>
-        <v>using, travel by_MISSING</v>
+        <v>using, travel_by_KGE-0A-50</v>
       </c>
       <c r="D64" s="65" t="str">
         <f t="shared" si="6"/>
-        <v>using, travel by_MISSING</v>
+        <v>using, travel_by_KGE-0A-50</v>
       </c>
       <c r="E64" s="64" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="F64" s="64" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="G64" s="64" t="s">
-        <v>265</v>
+        <v>267</v>
       </c>
       <c r="H64" s="4"/>
       <c r="I64" s="4"/>
@@ -5689,10 +5717,10 @@
     </row>
     <row r="65" ht="15.75" customHeight="1">
       <c r="A65" s="55" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="B65" s="56" t="s">
-        <v>267</v>
+        <v>269</v>
       </c>
       <c r="C65" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5703,13 +5731,13 @@
         <v>go_through_GID-102767 </v>
       </c>
       <c r="E65" s="56" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="F65" s="56" t="s">
-        <v>269</v>
+        <v>271</v>
       </c>
       <c r="G65" s="56" t="s">
-        <v>270</v>
+        <v>272</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4"/>
@@ -5735,10 +5763,10 @@
     </row>
     <row r="66" ht="15.75" customHeight="1">
       <c r="A66" s="55" t="s">
-        <v>271</v>
+        <v>273</v>
       </c>
       <c r="B66" s="56" t="s">
-        <v>272</v>
+        <v>274</v>
       </c>
       <c r="C66" s="57" t="str">
         <f t="shared" si="5"/>
@@ -5749,13 +5777,13 @@
         <v>serve_GID-97875</v>
       </c>
       <c r="E66" s="56" t="s">
-        <v>273</v>
+        <v>275</v>
       </c>
       <c r="F66" s="56" t="s">
-        <v>274</v>
+        <v>276</v>
       </c>
       <c r="G66" s="56" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4"/>
@@ -5780,16 +5808,29 @@
       <c r="AB66" s="4"/>
     </row>
     <row r="67" ht="15.75" customHeight="1">
-      <c r="A67" s="30"/>
-      <c r="B67" s="31"/>
-      <c r="C67" s="32"/>
-      <c r="D67" s="32" t="str">
+      <c r="A67" s="55" t="s">
+        <v>278</v>
+      </c>
+      <c r="B67" s="56" t="s">
+        <v>279</v>
+      </c>
+      <c r="C67" s="57" t="str">
+        <f t="shared" si="5"/>
+        <v>inside_UKC-106969 </v>
+      </c>
+      <c r="D67" s="57" t="str">
         <f t="shared" si="6"/>
-        <v/>
-      </c>
-      <c r="E67" s="31"/>
-      <c r="F67" s="31"/>
-      <c r="G67" s="31"/>
+        <v>inside_GID-106969 </v>
+      </c>
+      <c r="E67" s="56" t="s">
+        <v>280</v>
+      </c>
+      <c r="F67" s="56" t="s">
+        <v>281</v>
+      </c>
+      <c r="G67" s="56" t="s">
+        <v>282</v>
+      </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4"/>
       <c r="J67" s="4"/>
@@ -5814,7 +5855,7 @@
     </row>
     <row r="68" ht="15.75" customHeight="1">
       <c r="A68" s="5" t="s">
-        <v>276</v>
+        <v>283</v>
       </c>
       <c r="B68" s="6"/>
       <c r="C68" s="6"/>
@@ -5849,7 +5890,7 @@
       <c r="B69" s="67"/>
       <c r="C69" s="68"/>
       <c r="D69" s="68" t="s">
-        <v>277</v>
+        <v>284</v>
       </c>
       <c r="E69" s="7"/>
       <c r="F69" s="67"/>
@@ -5878,10 +5919,10 @@
     </row>
     <row r="70" ht="15.75" customHeight="1">
       <c r="A70" s="28" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="B70" s="21" t="s">
-        <v>279</v>
+        <v>286</v>
       </c>
       <c r="C70" s="15" t="str">
         <f t="shared" ref="C70:C102" si="7">B70&amp;"_"&amp;A70</f>
@@ -5892,13 +5933,13 @@
         <v>restaurant_GID-22077</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>280</v>
+        <v>287</v>
       </c>
       <c r="F70" s="21" t="s">
-        <v>281</v>
+        <v>288</v>
       </c>
       <c r="G70" s="21" t="s">
-        <v>282</v>
+        <v>289</v>
       </c>
       <c r="H70" s="4"/>
       <c r="I70" s="4"/>
@@ -5924,10 +5965,10 @@
     </row>
     <row r="71" ht="15.75" customHeight="1">
       <c r="A71" s="28" t="s">
-        <v>283</v>
+        <v>290</v>
       </c>
       <c r="B71" s="21" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="C71" s="15" t="str">
         <f t="shared" si="7"/>
@@ -5938,13 +5979,13 @@
         <v>bar_GID-14628 </v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>285</v>
+        <v>292</v>
       </c>
       <c r="F71" s="21" t="s">
-        <v>284</v>
+        <v>291</v>
       </c>
       <c r="G71" s="21" t="s">
-        <v>286</v>
+        <v>293</v>
       </c>
       <c r="H71" s="4"/>
       <c r="I71" s="4"/>
@@ -5970,10 +6011,10 @@
     </row>
     <row r="72" ht="15.75" customHeight="1">
       <c r="A72" s="28" t="s">
-        <v>287</v>
+        <v>294</v>
       </c>
       <c r="B72" s="21" t="s">
-        <v>288</v>
+        <v>295</v>
       </c>
       <c r="C72" s="15" t="str">
         <f t="shared" si="7"/>
@@ -5984,13 +6025,13 @@
         <v>university_GID-24619</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="F72" s="21" t="s">
-        <v>290</v>
+        <v>297</v>
       </c>
       <c r="G72" s="21" t="s">
-        <v>291</v>
+        <v>298</v>
       </c>
       <c r="H72" s="4"/>
       <c r="I72" s="4"/>
@@ -6016,10 +6057,10 @@
     </row>
     <row r="73" ht="15.75" customHeight="1">
       <c r="A73" s="28" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="B73" s="21" t="s">
-        <v>293</v>
+        <v>300</v>
       </c>
       <c r="C73" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6030,13 +6071,13 @@
         <v>supermarket_GID-23735</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>294</v>
+        <v>301</v>
       </c>
       <c r="F73" s="21" t="s">
-        <v>295</v>
+        <v>302</v>
       </c>
       <c r="G73" s="21" t="s">
-        <v>296</v>
+        <v>303</v>
       </c>
       <c r="H73" s="4"/>
       <c r="I73" s="4"/>
@@ -6062,10 +6103,10 @@
     </row>
     <row r="74" ht="15.75" customHeight="1">
       <c r="A74" s="28" t="s">
-        <v>297</v>
+        <v>304</v>
       </c>
       <c r="B74" s="21" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C74" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6076,13 +6117,13 @@
         <v>sport_facility_GID-18566</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>299</v>
+        <v>306</v>
       </c>
       <c r="F74" s="21" t="s">
-        <v>300</v>
+        <v>307</v>
       </c>
       <c r="G74" s="21" t="s">
-        <v>301</v>
+        <v>308</v>
       </c>
       <c r="H74" s="4"/>
       <c r="I74" s="4"/>
@@ -6108,10 +6149,10 @@
     </row>
     <row r="75" ht="15.75" customHeight="1">
       <c r="A75" s="28" t="s">
-        <v>302</v>
+        <v>309</v>
       </c>
       <c r="B75" s="21" t="s">
-        <v>303</v>
+        <v>310</v>
       </c>
       <c r="C75" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6122,13 +6163,13 @@
         <v>library_GID-19663</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>304</v>
+        <v>311</v>
       </c>
       <c r="F75" s="21" t="s">
-        <v>305</v>
+        <v>312</v>
       </c>
       <c r="G75" s="21" t="s">
-        <v>306</v>
+        <v>313</v>
       </c>
       <c r="H75" s="4"/>
       <c r="I75" s="4"/>
@@ -6154,10 +6195,10 @@
     </row>
     <row r="76" ht="15.75" customHeight="1">
       <c r="A76" s="28" t="s">
-        <v>307</v>
+        <v>314</v>
       </c>
       <c r="B76" s="21" t="s">
-        <v>308</v>
+        <v>315</v>
       </c>
       <c r="C76" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6168,13 +6209,13 @@
         <v>student_accommodation, dorm_GID-17139</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>309</v>
+        <v>316</v>
       </c>
       <c r="F76" s="21" t="s">
-        <v>310</v>
+        <v>317</v>
       </c>
       <c r="G76" s="21" t="s">
-        <v>311</v>
+        <v>318</v>
       </c>
       <c r="H76" s="4"/>
       <c r="I76" s="4"/>
@@ -6200,10 +6241,10 @@
     </row>
     <row r="77" ht="15.75" customHeight="1">
       <c r="A77" s="28" t="s">
-        <v>312</v>
+        <v>319</v>
       </c>
       <c r="B77" s="21" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="C77" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6214,13 +6255,13 @@
         <v>hotel_GID-18979</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>314</v>
+        <v>321</v>
       </c>
       <c r="F77" s="21" t="s">
-        <v>313</v>
+        <v>320</v>
       </c>
       <c r="G77" s="21" t="s">
-        <v>315</v>
+        <v>322</v>
       </c>
       <c r="H77" s="4"/>
       <c r="I77" s="4"/>
@@ -6246,10 +6287,10 @@
     </row>
     <row r="78" ht="15.75" customHeight="1">
       <c r="A78" s="28" t="s">
-        <v>316</v>
+        <v>323</v>
       </c>
       <c r="B78" s="21" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="C78" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6260,13 +6301,13 @@
         <v>pizzeria_GID-21345</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>318</v>
+        <v>325</v>
       </c>
       <c r="F78" s="21" t="s">
-        <v>317</v>
+        <v>324</v>
       </c>
       <c r="G78" s="21" t="s">
-        <v>319</v>
+        <v>326</v>
       </c>
       <c r="H78" s="4"/>
       <c r="I78" s="4"/>
@@ -6292,10 +6333,10 @@
     </row>
     <row r="79" ht="15.75" customHeight="1">
       <c r="A79" s="28" t="s">
-        <v>320</v>
+        <v>327</v>
       </c>
       <c r="B79" s="21" t="s">
-        <v>321</v>
+        <v>328</v>
       </c>
       <c r="C79" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6306,13 +6347,13 @@
         <v>sports_field_GID-45304</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>322</v>
+        <v>329</v>
       </c>
       <c r="F79" s="21" t="s">
-        <v>323</v>
+        <v>330</v>
       </c>
       <c r="G79" s="21" t="s">
-        <v>324</v>
+        <v>331</v>
       </c>
       <c r="H79" s="4"/>
       <c r="I79" s="4"/>
@@ -6338,10 +6379,10 @@
     </row>
     <row r="80" ht="15.75" customHeight="1">
       <c r="A80" s="28" t="s">
-        <v>325</v>
+        <v>332</v>
       </c>
       <c r="B80" s="21" t="s">
-        <v>326</v>
+        <v>333</v>
       </c>
       <c r="C80" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6352,13 +6393,13 @@
         <v>pharmacy_GID-17277</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>327</v>
+        <v>334</v>
       </c>
       <c r="F80" s="21" t="s">
-        <v>328</v>
+        <v>335</v>
       </c>
       <c r="G80" s="21" t="s">
-        <v>329</v>
+        <v>336</v>
       </c>
       <c r="H80" s="4"/>
       <c r="I80" s="4"/>
@@ -6384,10 +6425,10 @@
     </row>
     <row r="81" ht="15.75" customHeight="1">
       <c r="A81" s="28" t="s">
-        <v>330</v>
+        <v>337</v>
       </c>
       <c r="B81" s="21" t="s">
-        <v>331</v>
+        <v>338</v>
       </c>
       <c r="C81" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6398,13 +6439,13 @@
         <v>bank_GID-14574</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>332</v>
+        <v>339</v>
       </c>
       <c r="F81" s="21" t="s">
-        <v>333</v>
+        <v>340</v>
       </c>
       <c r="G81" s="21" t="s">
-        <v>334</v>
+        <v>341</v>
       </c>
       <c r="H81" s="4"/>
       <c r="I81" s="4"/>
@@ -6430,10 +6471,10 @@
     </row>
     <row r="82" ht="15.75" customHeight="1">
       <c r="A82" s="28" t="s">
-        <v>335</v>
+        <v>342</v>
       </c>
       <c r="B82" s="21" t="s">
-        <v>336</v>
+        <v>343</v>
       </c>
       <c r="C82" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6444,13 +6485,13 @@
         <v>dentist, dental office_KGE24-0A-28</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>337</v>
+        <v>344</v>
       </c>
       <c r="F82" s="21" t="s">
-        <v>338</v>
+        <v>345</v>
       </c>
       <c r="G82" s="21" t="s">
-        <v>339</v>
+        <v>346</v>
       </c>
       <c r="H82" s="4"/>
       <c r="I82" s="4"/>
@@ -6476,10 +6517,10 @@
     </row>
     <row r="83" ht="15.75" customHeight="1">
       <c r="A83" s="28" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="B83" s="21" t="s">
-        <v>341</v>
+        <v>348</v>
       </c>
       <c r="C83" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6490,13 +6531,13 @@
         <v>train_station_GID-21898</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>342</v>
+        <v>349</v>
       </c>
       <c r="F83" s="21" t="s">
-        <v>343</v>
+        <v>350</v>
       </c>
       <c r="G83" s="21" t="s">
-        <v>344</v>
+        <v>351</v>
       </c>
       <c r="H83" s="4"/>
       <c r="I83" s="4"/>
@@ -6522,10 +6563,10 @@
     </row>
     <row r="84" ht="15.75" customHeight="1">
       <c r="A84" s="28" t="s">
-        <v>340</v>
+        <v>347</v>
       </c>
       <c r="B84" s="21" t="s">
-        <v>345</v>
+        <v>352</v>
       </c>
       <c r="C84" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6536,13 +6577,13 @@
         <v>health_service_GID-21898</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>346</v>
+        <v>353</v>
       </c>
       <c r="F84" s="21" t="s">
-        <v>347</v>
+        <v>354</v>
       </c>
       <c r="G84" s="21" t="s">
-        <v>348</v>
+        <v>355</v>
       </c>
       <c r="H84" s="4"/>
       <c r="I84" s="4"/>
@@ -6568,10 +6609,10 @@
     </row>
     <row r="85" ht="15.75" customHeight="1">
       <c r="A85" s="28" t="s">
-        <v>349</v>
+        <v>356</v>
       </c>
       <c r="B85" s="21" t="s">
-        <v>350</v>
+        <v>357</v>
       </c>
       <c r="C85" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6582,13 +6623,13 @@
         <v>hairdresser_GID-22377</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>351</v>
+        <v>358</v>
       </c>
       <c r="F85" s="21" t="s">
-        <v>352</v>
+        <v>359</v>
       </c>
       <c r="G85" s="21" t="s">
-        <v>353</v>
+        <v>360</v>
       </c>
       <c r="H85" s="4"/>
       <c r="I85" s="4"/>
@@ -6614,10 +6655,10 @@
     </row>
     <row r="86" ht="15.75" customHeight="1">
       <c r="A86" s="28" t="s">
-        <v>354</v>
+        <v>361</v>
       </c>
       <c r="B86" s="21" t="s">
-        <v>355</v>
+        <v>362</v>
       </c>
       <c r="C86" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6628,13 +6669,13 @@
         <v>jewelry_store_GID-42955</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>356</v>
+        <v>363</v>
       </c>
       <c r="F86" s="21" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="G86" s="21" t="s">
-        <v>358</v>
+        <v>365</v>
       </c>
       <c r="H86" s="4"/>
       <c r="I86" s="4"/>
@@ -6660,10 +6701,10 @@
     </row>
     <row r="87" ht="15.75" customHeight="1">
       <c r="A87" s="28" t="s">
-        <v>359</v>
+        <v>366</v>
       </c>
       <c r="B87" s="21" t="s">
-        <v>360</v>
+        <v>367</v>
       </c>
       <c r="C87" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6674,13 +6715,13 @@
         <v>monument_GID-45446</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>361</v>
+        <v>368</v>
       </c>
       <c r="F87" s="21" t="s">
-        <v>362</v>
+        <v>369</v>
       </c>
       <c r="G87" s="21" t="s">
-        <v>363</v>
+        <v>370</v>
       </c>
       <c r="H87" s="4"/>
       <c r="I87" s="4"/>
@@ -6706,10 +6747,10 @@
     </row>
     <row r="88" ht="15.75" customHeight="1">
       <c r="A88" s="28" t="s">
-        <v>364</v>
+        <v>371</v>
       </c>
       <c r="B88" s="21" t="s">
-        <v>365</v>
+        <v>372</v>
       </c>
       <c r="C88" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6720,13 +6761,13 @@
         <v>museum_GID-20454</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>366</v>
+        <v>373</v>
       </c>
       <c r="F88" s="21" t="s">
-        <v>367</v>
+        <v>374</v>
       </c>
       <c r="G88" s="21" t="s">
-        <v>368</v>
+        <v>375</v>
       </c>
       <c r="H88" s="4"/>
       <c r="I88" s="4"/>
@@ -6752,10 +6793,10 @@
     </row>
     <row r="89" ht="15.75" customHeight="1">
       <c r="A89" s="28" t="s">
-        <v>369</v>
+        <v>376</v>
       </c>
       <c r="B89" s="21" t="s">
-        <v>370</v>
+        <v>377</v>
       </c>
       <c r="C89" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6766,13 +6807,13 @@
         <v>shop_GID-22782</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>371</v>
+        <v>378</v>
       </c>
       <c r="F89" s="21" t="s">
-        <v>372</v>
+        <v>379</v>
       </c>
       <c r="G89" s="21" t="s">
-        <v>373</v>
+        <v>380</v>
       </c>
       <c r="H89" s="4"/>
       <c r="I89" s="4"/>
@@ -6798,10 +6839,10 @@
     </row>
     <row r="90" ht="15.75" customHeight="1">
       <c r="A90" s="28" t="s">
-        <v>374</v>
+        <v>381</v>
       </c>
       <c r="B90" s="21" t="s">
-        <v>375</v>
+        <v>382</v>
       </c>
       <c r="C90" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6812,13 +6853,13 @@
         <v>ice_cream_shop_pastry_shop, milk_bar_GID-20240</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>376</v>
+        <v>383</v>
       </c>
       <c r="F90" s="21" t="s">
-        <v>377</v>
+        <v>384</v>
       </c>
       <c r="G90" s="21" t="s">
-        <v>378</v>
+        <v>385</v>
       </c>
       <c r="H90" s="4"/>
       <c r="I90" s="4"/>
@@ -6844,10 +6885,10 @@
     </row>
     <row r="91" ht="15.75" customHeight="1">
       <c r="A91" s="28" t="s">
-        <v>379</v>
+        <v>386</v>
       </c>
       <c r="B91" s="21" t="s">
-        <v>380</v>
+        <v>387</v>
       </c>
       <c r="C91" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6858,13 +6899,13 @@
         <v>post_office_GID-110273</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>381</v>
+        <v>388</v>
       </c>
       <c r="F91" s="21" t="s">
-        <v>382</v>
+        <v>389</v>
       </c>
       <c r="G91" s="21" t="s">
-        <v>383</v>
+        <v>390</v>
       </c>
       <c r="H91" s="4"/>
       <c r="I91" s="4"/>
@@ -6890,10 +6931,10 @@
     </row>
     <row r="92" ht="15.75" customHeight="1">
       <c r="A92" s="28" t="s">
-        <v>384</v>
+        <v>391</v>
       </c>
       <c r="B92" s="21" t="s">
-        <v>385</v>
+        <v>392</v>
       </c>
       <c r="C92" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6904,13 +6945,13 @@
         <v>beer_shop_GID-23949</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>386</v>
+        <v>393</v>
       </c>
       <c r="F92" s="21" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="G92" s="21" t="s">
-        <v>388</v>
+        <v>395</v>
       </c>
       <c r="H92" s="4"/>
       <c r="I92" s="4"/>
@@ -6936,10 +6977,10 @@
     </row>
     <row r="93" ht="15.75" customHeight="1">
       <c r="A93" s="28" t="s">
-        <v>389</v>
+        <v>396</v>
       </c>
       <c r="B93" s="21" t="s">
-        <v>390</v>
+        <v>397</v>
       </c>
       <c r="C93" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6950,13 +6991,13 @@
         <v>stationery_bookstore_GID-15080</v>
       </c>
       <c r="E93" s="21" t="s">
-        <v>391</v>
+        <v>398</v>
       </c>
       <c r="F93" s="21" t="s">
-        <v>392</v>
+        <v>399</v>
       </c>
       <c r="G93" s="21" t="s">
-        <v>393</v>
+        <v>400</v>
       </c>
       <c r="H93" s="4"/>
       <c r="I93" s="4"/>
@@ -6982,10 +7023,10 @@
     </row>
     <row r="94" ht="15.75" customHeight="1">
       <c r="A94" s="28" t="s">
-        <v>394</v>
+        <v>401</v>
       </c>
       <c r="B94" s="21" t="s">
-        <v>395</v>
+        <v>402</v>
       </c>
       <c r="C94" s="15" t="str">
         <f t="shared" si="7"/>
@@ -6996,13 +7037,13 @@
         <v>bus_station_GID-15406</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>396</v>
+        <v>403</v>
       </c>
       <c r="F94" s="70" t="s">
-        <v>397</v>
+        <v>404</v>
       </c>
       <c r="G94" s="21" t="s">
-        <v>398</v>
+        <v>405</v>
       </c>
       <c r="H94" s="4"/>
       <c r="I94" s="4"/>
@@ -7028,10 +7069,10 @@
     </row>
     <row r="95" ht="15.75" customHeight="1">
       <c r="A95" s="28" t="s">
-        <v>399</v>
+        <v>406</v>
       </c>
       <c r="B95" s="21" t="s">
-        <v>400</v>
+        <v>407</v>
       </c>
       <c r="C95" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7042,13 +7083,13 @@
         <v>parking_space_GID-45482</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>401</v>
+        <v>408</v>
       </c>
       <c r="F95" s="21" t="s">
-        <v>402</v>
+        <v>409</v>
       </c>
       <c r="G95" s="21" t="s">
-        <v>403</v>
+        <v>410</v>
       </c>
       <c r="H95" s="4"/>
       <c r="I95" s="4"/>
@@ -7074,10 +7115,10 @@
     </row>
     <row r="96" ht="15.75" customHeight="1">
       <c r="A96" s="28" t="s">
-        <v>404</v>
+        <v>411</v>
       </c>
       <c r="B96" s="21" t="s">
-        <v>405</v>
+        <v>412</v>
       </c>
       <c r="C96" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7088,13 +7129,13 @@
         <v>tobacco_shop_GID-24229</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>406</v>
+        <v>413</v>
       </c>
       <c r="F96" s="21" t="s">
-        <v>407</v>
+        <v>414</v>
       </c>
       <c r="G96" s="21" t="s">
-        <v>408</v>
+        <v>415</v>
       </c>
       <c r="H96" s="4"/>
       <c r="I96" s="4"/>
@@ -7120,10 +7161,10 @@
     </row>
     <row r="97" ht="15.75" customHeight="1">
       <c r="A97" s="28" t="s">
-        <v>409</v>
+        <v>416</v>
       </c>
       <c r="B97" s="21" t="s">
-        <v>410</v>
+        <v>417</v>
       </c>
       <c r="C97" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7134,13 +7175,13 @@
         <v>market_GID-44731</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>411</v>
+        <v>418</v>
       </c>
       <c r="F97" s="21" t="s">
-        <v>412</v>
+        <v>419</v>
       </c>
       <c r="G97" s="21" t="s">
-        <v>413</v>
+        <v>420</v>
       </c>
       <c r="H97" s="4"/>
       <c r="I97" s="4"/>
@@ -7166,10 +7207,10 @@
     </row>
     <row r="98" ht="15.75" customHeight="1">
       <c r="A98" s="28" t="s">
-        <v>414</v>
+        <v>421</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>415</v>
+        <v>422</v>
       </c>
       <c r="C98" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7180,13 +7221,13 @@
         <v>hospital_GID-18969</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>416</v>
+        <v>423</v>
       </c>
       <c r="F98" s="21" t="s">
-        <v>417</v>
+        <v>424</v>
       </c>
       <c r="G98" s="21" t="s">
-        <v>418</v>
+        <v>425</v>
       </c>
       <c r="H98" s="4"/>
       <c r="I98" s="4"/>
@@ -7212,10 +7253,10 @@
     </row>
     <row r="99" ht="15.75" customHeight="1">
       <c r="A99" s="28" t="s">
-        <v>419</v>
+        <v>426</v>
       </c>
       <c r="B99" s="21" t="s">
-        <v>420</v>
+        <v>427</v>
       </c>
       <c r="C99" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7226,13 +7267,13 @@
         <v>cabelcar_GID-24016</v>
       </c>
       <c r="E99" s="21" t="s">
-        <v>421</v>
+        <v>428</v>
       </c>
       <c r="F99" s="21" t="s">
-        <v>422</v>
+        <v>429</v>
       </c>
       <c r="G99" s="21" t="s">
-        <v>423</v>
+        <v>430</v>
       </c>
       <c r="H99" s="4"/>
       <c r="I99" s="4"/>
@@ -7258,10 +7299,10 @@
     </row>
     <row r="100" ht="15.75" customHeight="1">
       <c r="A100" s="28" t="s">
-        <v>424</v>
+        <v>431</v>
       </c>
       <c r="B100" s="21" t="s">
-        <v>425</v>
+        <v>432</v>
       </c>
       <c r="C100" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7272,13 +7313,13 @@
         <v>grocery store_GID-18499</v>
       </c>
       <c r="E100" s="21" t="s">
-        <v>426</v>
+        <v>433</v>
       </c>
       <c r="F100" s="21" t="s">
-        <v>427</v>
+        <v>434</v>
       </c>
       <c r="G100" s="21" t="s">
-        <v>428</v>
+        <v>435</v>
       </c>
       <c r="H100" s="4"/>
       <c r="I100" s="4"/>
@@ -7304,10 +7345,10 @@
     </row>
     <row r="101" ht="15.75" customHeight="1">
       <c r="A101" s="28" t="s">
-        <v>429</v>
+        <v>436</v>
       </c>
       <c r="B101" s="21" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="C101" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7318,13 +7359,13 @@
         <v>bedbreakfast_GID-14768</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>431</v>
+        <v>438</v>
       </c>
       <c r="F101" s="21" t="s">
-        <v>430</v>
+        <v>437</v>
       </c>
       <c r="G101" s="21" t="s">
-        <v>432</v>
+        <v>439</v>
       </c>
       <c r="H101" s="4"/>
       <c r="I101" s="4"/>
@@ -7350,10 +7391,10 @@
     </row>
     <row r="102" ht="15.75" customHeight="1">
       <c r="A102" s="28" t="s">
-        <v>433</v>
+        <v>440</v>
       </c>
       <c r="B102" s="21" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="C102" s="15" t="str">
         <f t="shared" si="7"/>
@@ -7364,13 +7405,13 @@
         <v>fast_food_GID-39991</v>
       </c>
       <c r="E102" s="21" t="s">
-        <v>435</v>
+        <v>442</v>
       </c>
       <c r="F102" s="21" t="s">
-        <v>434</v>
+        <v>441</v>
       </c>
       <c r="G102" s="21" t="s">
-        <v>436</v>
+        <v>443</v>
       </c>
       <c r="H102" s="4"/>
       <c r="I102" s="4"/>
@@ -7396,26 +7437,26 @@
     </row>
     <row r="103" ht="15.75" customHeight="1">
       <c r="A103" s="28" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="B103" s="21" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="C103" s="71" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="D103" s="15" t="str">
         <f t="shared" si="8"/>
         <v>appartamento</v>
       </c>
       <c r="E103" s="21" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
       <c r="F103" s="21" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="G103" s="21" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="H103" s="4"/>
       <c r="I103" s="4"/>
@@ -7441,10 +7482,10 @@
     </row>
     <row r="104" ht="15.75" customHeight="1">
       <c r="A104" s="28" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
       <c r="B104" s="21" t="s">
-        <v>443</v>
+        <v>450</v>
       </c>
       <c r="C104" s="15" t="str">
         <f t="shared" ref="C104:C127" si="9">B104&amp;"_"&amp;A104</f>
@@ -7455,13 +7496,13 @@
         <v>internet-point_KGE24-0A-35</v>
       </c>
       <c r="E104" s="21" t="s">
-        <v>444</v>
+        <v>451</v>
       </c>
       <c r="F104" s="21" t="s">
-        <v>445</v>
+        <v>452</v>
       </c>
       <c r="G104" s="21" t="s">
-        <v>446</v>
+        <v>453</v>
       </c>
       <c r="H104" s="4"/>
       <c r="I104" s="4"/>
@@ -7487,10 +7528,10 @@
     </row>
     <row r="105" ht="15.75" customHeight="1">
       <c r="A105" s="28" t="s">
-        <v>447</v>
+        <v>454</v>
       </c>
       <c r="B105" s="21" t="s">
-        <v>448</v>
+        <v>455</v>
       </c>
       <c r="C105" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7501,13 +7542,13 @@
         <v>souvenir_shop_KGE24-0A-36</v>
       </c>
       <c r="E105" s="21" t="s">
-        <v>449</v>
+        <v>456</v>
       </c>
       <c r="F105" s="21" t="s">
-        <v>450</v>
+        <v>457</v>
       </c>
       <c r="G105" s="21" t="s">
-        <v>451</v>
+        <v>458</v>
       </c>
       <c r="H105" s="4"/>
       <c r="I105" s="4"/>
@@ -7533,10 +7574,10 @@
     </row>
     <row r="106" ht="15.75" customHeight="1">
       <c r="A106" s="28" t="s">
-        <v>452</v>
+        <v>459</v>
       </c>
       <c r="B106" s="21" t="s">
-        <v>453</v>
+        <v>460</v>
       </c>
       <c r="C106" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7547,13 +7588,13 @@
         <v>clothin_store_KGE24-0A-37</v>
       </c>
       <c r="E106" s="21" t="s">
-        <v>454</v>
+        <v>461</v>
       </c>
       <c r="F106" s="21" t="s">
-        <v>455</v>
+        <v>462</v>
       </c>
       <c r="G106" s="21" t="s">
-        <v>456</v>
+        <v>463</v>
       </c>
       <c r="H106" s="4"/>
       <c r="I106" s="4"/>
@@ -7579,10 +7620,10 @@
     </row>
     <row r="107" ht="15.75" customHeight="1">
       <c r="A107" s="28" t="s">
-        <v>457</v>
+        <v>464</v>
       </c>
       <c r="B107" s="21" t="s">
-        <v>458</v>
+        <v>465</v>
       </c>
       <c r="C107" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7593,13 +7634,13 @@
         <v>bank_branch_KGE24-0A-38</v>
       </c>
       <c r="E107" s="21" t="s">
-        <v>459</v>
+        <v>466</v>
       </c>
       <c r="F107" s="21" t="s">
-        <v>460</v>
+        <v>467</v>
       </c>
       <c r="G107" s="21" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="H107" s="4"/>
       <c r="I107" s="4"/>
@@ -7625,10 +7666,10 @@
     </row>
     <row r="108" ht="15.75" customHeight="1">
       <c r="A108" s="28" t="s">
-        <v>462</v>
+        <v>469</v>
       </c>
       <c r="B108" s="21" t="s">
-        <v>463</v>
+        <v>470</v>
       </c>
       <c r="C108" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7639,13 +7680,13 @@
         <v>typical_product_store_KGE24-0A-39</v>
       </c>
       <c r="E108" s="70" t="s">
-        <v>464</v>
+        <v>471</v>
       </c>
       <c r="F108" s="21" t="s">
-        <v>465</v>
+        <v>472</v>
       </c>
       <c r="G108" s="21" t="s">
-        <v>466</v>
+        <v>473</v>
       </c>
       <c r="H108" s="4"/>
       <c r="I108" s="4"/>
@@ -7671,10 +7712,10 @@
     </row>
     <row r="109" ht="15.75" customHeight="1">
       <c r="A109" s="28" t="s">
-        <v>467</v>
+        <v>474</v>
       </c>
       <c r="B109" s="21" t="s">
-        <v>468</v>
+        <v>475</v>
       </c>
       <c r="C109" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7685,13 +7726,13 @@
         <v>ski_rental_KGE24-0A-40</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="F109" s="21" t="s">
-        <v>470</v>
+        <v>477</v>
       </c>
       <c r="G109" s="21" t="s">
-        <v>469</v>
+        <v>476</v>
       </c>
       <c r="H109" s="4"/>
       <c r="I109" s="4"/>
@@ -7717,10 +7758,10 @@
     </row>
     <row r="110" ht="15.75" customHeight="1">
       <c r="A110" s="28" t="s">
-        <v>471</v>
+        <v>478</v>
       </c>
       <c r="B110" s="21" t="s">
-        <v>472</v>
+        <v>479</v>
       </c>
       <c r="C110" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7731,13 +7772,13 @@
         <v>electronics store_KGE24-0A-41</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>473</v>
+        <v>480</v>
       </c>
       <c r="F110" s="21" t="s">
-        <v>474</v>
+        <v>481</v>
       </c>
       <c r="G110" s="21" t="s">
-        <v>475</v>
+        <v>482</v>
       </c>
       <c r="H110" s="4"/>
       <c r="I110" s="4"/>
@@ -7763,10 +7804,10 @@
     </row>
     <row r="111" ht="15.75" customHeight="1">
       <c r="A111" s="28" t="s">
-        <v>476</v>
+        <v>483</v>
       </c>
       <c r="B111" s="21" t="s">
-        <v>477</v>
+        <v>484</v>
       </c>
       <c r="C111" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7777,13 +7818,13 @@
         <v>perfumery_GID-21134</v>
       </c>
       <c r="E111" s="21" t="s">
-        <v>478</v>
+        <v>485</v>
       </c>
       <c r="F111" s="21" t="s">
-        <v>479</v>
+        <v>486</v>
       </c>
       <c r="G111" s="21" t="s">
-        <v>480</v>
+        <v>487</v>
       </c>
       <c r="H111" s="4"/>
       <c r="I111" s="4"/>
@@ -7809,10 +7850,10 @@
     </row>
     <row r="112" ht="15.75" customHeight="1">
       <c r="A112" s="28" t="s">
-        <v>481</v>
+        <v>488</v>
       </c>
       <c r="B112" s="21" t="s">
-        <v>482</v>
+        <v>489</v>
       </c>
       <c r="C112" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7823,13 +7864,13 @@
         <v>health club_GID-18769</v>
       </c>
       <c r="E112" s="21" t="s">
-        <v>483</v>
+        <v>490</v>
       </c>
       <c r="F112" s="21" t="s">
-        <v>484</v>
+        <v>491</v>
       </c>
       <c r="G112" s="21" t="s">
-        <v>485</v>
+        <v>492</v>
       </c>
       <c r="H112" s="4"/>
       <c r="I112" s="4"/>
@@ -7855,10 +7896,10 @@
     </row>
     <row r="113" ht="15.75" customHeight="1">
       <c r="A113" s="28" t="s">
-        <v>486</v>
+        <v>493</v>
       </c>
       <c r="B113" s="21" t="s">
-        <v>487</v>
+        <v>494</v>
       </c>
       <c r="C113" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7869,13 +7910,13 @@
         <v>shopping_mall_GID-21414</v>
       </c>
       <c r="E113" s="21" t="s">
-        <v>488</v>
+        <v>495</v>
       </c>
       <c r="F113" s="21" t="s">
-        <v>489</v>
+        <v>496</v>
       </c>
       <c r="G113" s="21" t="s">
-        <v>490</v>
+        <v>497</v>
       </c>
       <c r="H113" s="4"/>
       <c r="I113" s="4"/>
@@ -7901,10 +7942,10 @@
     </row>
     <row r="114" ht="15.75" customHeight="1">
       <c r="A114" s="28" t="s">
-        <v>491</v>
+        <v>498</v>
       </c>
       <c r="B114" s="21" t="s">
-        <v>492</v>
+        <v>499</v>
       </c>
       <c r="C114" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7915,13 +7956,13 @@
         <v>swimming_pool_GID-23807</v>
       </c>
       <c r="E114" s="21" t="s">
-        <v>493</v>
+        <v>500</v>
       </c>
       <c r="F114" s="21" t="s">
-        <v>494</v>
+        <v>501</v>
       </c>
       <c r="G114" s="21" t="s">
-        <v>495</v>
+        <v>502</v>
       </c>
       <c r="H114" s="4"/>
       <c r="I114" s="4"/>
@@ -7947,10 +7988,10 @@
     </row>
     <row r="115" ht="15.75" customHeight="1">
       <c r="A115" s="28" t="s">
-        <v>496</v>
+        <v>503</v>
       </c>
       <c r="B115" s="21" t="s">
-        <v>497</v>
+        <v>504</v>
       </c>
       <c r="C115" s="15" t="str">
         <f t="shared" si="9"/>
@@ -7961,13 +8002,13 @@
         <v>camping site_GID-45121</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>498</v>
+        <v>505</v>
       </c>
       <c r="F115" s="21" t="s">
-        <v>499</v>
+        <v>506</v>
       </c>
       <c r="G115" s="21" t="s">
-        <v>500</v>
+        <v>507</v>
       </c>
       <c r="H115" s="4"/>
       <c r="I115" s="4"/>
@@ -7993,10 +8034,10 @@
     </row>
     <row r="116" ht="15.75" customHeight="1">
       <c r="A116" s="28" t="s">
-        <v>501</v>
+        <v>508</v>
       </c>
       <c r="B116" s="21" t="s">
-        <v>502</v>
+        <v>509</v>
       </c>
       <c r="C116" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8007,13 +8048,13 @@
         <v>theatre_GID-24081</v>
       </c>
       <c r="E116" s="21" t="s">
-        <v>503</v>
+        <v>510</v>
       </c>
       <c r="F116" s="21" t="s">
-        <v>504</v>
+        <v>511</v>
       </c>
       <c r="G116" s="21" t="s">
-        <v>505</v>
+        <v>512</v>
       </c>
       <c r="H116" s="4"/>
       <c r="I116" s="4"/>
@@ -8039,10 +8080,10 @@
     </row>
     <row r="117" ht="15.75" customHeight="1">
       <c r="A117" s="28" t="s">
-        <v>506</v>
+        <v>513</v>
       </c>
       <c r="B117" s="21" t="s">
-        <v>507</v>
+        <v>514</v>
       </c>
       <c r="C117" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8053,13 +8094,13 @@
         <v>nightclub_GID-15442</v>
       </c>
       <c r="E117" s="21" t="s">
-        <v>508</v>
+        <v>515</v>
       </c>
       <c r="F117" s="21" t="s">
-        <v>509</v>
+        <v>516</v>
       </c>
       <c r="G117" s="21" t="s">
-        <v>510</v>
+        <v>517</v>
       </c>
       <c r="H117" s="4"/>
       <c r="I117" s="4"/>
@@ -8085,10 +8126,10 @@
     </row>
     <row r="118" ht="15.75" customHeight="1">
       <c r="A118" s="28" t="s">
-        <v>511</v>
+        <v>518</v>
       </c>
       <c r="B118" s="21" t="s">
-        <v>512</v>
+        <v>519</v>
       </c>
       <c r="C118" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8099,13 +8140,13 @@
         <v>ice_stadium_GID-22152</v>
       </c>
       <c r="E118" s="21" t="s">
-        <v>513</v>
+        <v>520</v>
       </c>
       <c r="F118" s="21" t="s">
-        <v>514</v>
+        <v>521</v>
       </c>
       <c r="G118" s="21" t="s">
-        <v>515</v>
+        <v>522</v>
       </c>
       <c r="H118" s="4"/>
       <c r="I118" s="4"/>
@@ -8131,10 +8172,10 @@
     </row>
     <row r="119" ht="15.75" customHeight="1">
       <c r="A119" s="28" t="s">
-        <v>516</v>
+        <v>523</v>
       </c>
       <c r="B119" s="21" t="s">
-        <v>517</v>
+        <v>524</v>
       </c>
       <c r="C119" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8145,13 +8186,13 @@
         <v>residence_GID-45262</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>518</v>
+        <v>525</v>
       </c>
       <c r="F119" s="21" t="s">
-        <v>519</v>
+        <v>526</v>
       </c>
       <c r="G119" s="21" t="s">
-        <v>520</v>
+        <v>527</v>
       </c>
       <c r="H119" s="4"/>
       <c r="I119" s="4"/>
@@ -8177,10 +8218,10 @@
     </row>
     <row r="120" ht="15.75" customHeight="1">
       <c r="A120" s="28" t="s">
-        <v>521</v>
+        <v>528</v>
       </c>
       <c r="B120" s="21" t="s">
-        <v>522</v>
+        <v>529</v>
       </c>
       <c r="C120" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8191,13 +8232,13 @@
         <v>stationery_shop_KGE24-0A-42</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>523</v>
+        <v>530</v>
       </c>
       <c r="F120" s="21" t="s">
-        <v>524</v>
+        <v>531</v>
       </c>
       <c r="G120" s="21" t="s">
-        <v>525</v>
+        <v>532</v>
       </c>
       <c r="H120" s="4"/>
       <c r="I120" s="4"/>
@@ -8223,10 +8264,10 @@
     </row>
     <row r="121" ht="15.75" customHeight="1">
       <c r="A121" s="28" t="s">
-        <v>526</v>
+        <v>533</v>
       </c>
       <c r="B121" s="21" t="s">
-        <v>527</v>
+        <v>534</v>
       </c>
       <c r="C121" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8237,13 +8278,13 @@
         <v>jewellry_store_KGE24-0A-43</v>
       </c>
       <c r="E121" s="21" t="s">
-        <v>528</v>
+        <v>535</v>
       </c>
       <c r="F121" s="21" t="s">
-        <v>357</v>
+        <v>364</v>
       </c>
       <c r="G121" s="21" t="s">
-        <v>529</v>
+        <v>536</v>
       </c>
       <c r="H121" s="4"/>
       <c r="I121" s="4"/>
@@ -8269,10 +8310,10 @@
     </row>
     <row r="122" ht="15.75" customHeight="1">
       <c r="A122" s="28" t="s">
-        <v>530</v>
+        <v>537</v>
       </c>
       <c r="B122" s="21" t="s">
-        <v>531</v>
+        <v>538</v>
       </c>
       <c r="C122" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8283,13 +8324,13 @@
         <v>pet_store_KGE24-0A-44</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>532</v>
+        <v>539</v>
       </c>
       <c r="F122" s="21" t="s">
-        <v>533</v>
+        <v>540</v>
       </c>
       <c r="G122" s="21" t="s">
-        <v>534</v>
+        <v>541</v>
       </c>
       <c r="H122" s="4"/>
       <c r="I122" s="4"/>
@@ -8315,10 +8356,10 @@
     </row>
     <row r="123" ht="15.75" customHeight="1">
       <c r="A123" s="28" t="s">
-        <v>535</v>
+        <v>542</v>
       </c>
       <c r="B123" s="21" t="s">
-        <v>536</v>
+        <v>543</v>
       </c>
       <c r="C123" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8329,13 +8370,13 @@
         <v>farmhouse_GID-17664</v>
       </c>
       <c r="E123" s="21" t="s">
-        <v>537</v>
+        <v>544</v>
       </c>
       <c r="F123" s="21" t="s">
-        <v>538</v>
+        <v>545</v>
       </c>
       <c r="G123" s="21" t="s">
-        <v>539</v>
+        <v>546</v>
       </c>
       <c r="H123" s="4"/>
       <c r="I123" s="4"/>
@@ -8361,10 +8402,10 @@
     </row>
     <row r="124" ht="15.75" customHeight="1">
       <c r="A124" s="28" t="s">
-        <v>540</v>
+        <v>547</v>
       </c>
       <c r="B124" s="21" t="s">
-        <v>541</v>
+        <v>548</v>
       </c>
       <c r="C124" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8375,13 +8416,13 @@
         <v>dairy_KGE24-0A-45</v>
       </c>
       <c r="E124" s="21" t="s">
-        <v>542</v>
+        <v>549</v>
       </c>
       <c r="F124" s="21" t="s">
-        <v>543</v>
+        <v>550</v>
       </c>
       <c r="G124" s="21" t="s">
-        <v>544</v>
+        <v>551</v>
       </c>
       <c r="H124" s="4"/>
       <c r="I124" s="4"/>
@@ -8407,10 +8448,10 @@
     </row>
     <row r="125" ht="15.75" customHeight="1">
       <c r="A125" s="28" t="s">
-        <v>545</v>
+        <v>552</v>
       </c>
       <c r="B125" s="21" t="s">
-        <v>546</v>
+        <v>553</v>
       </c>
       <c r="C125" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8421,13 +8462,13 @@
         <v>sports store_KGE24-0A-46</v>
       </c>
       <c r="E125" s="21" t="s">
-        <v>547</v>
+        <v>554</v>
       </c>
       <c r="F125" s="21" t="s">
-        <v>548</v>
+        <v>555</v>
       </c>
       <c r="G125" s="21" t="s">
-        <v>549</v>
+        <v>556</v>
       </c>
       <c r="H125" s="4"/>
       <c r="I125" s="4"/>
@@ -8453,10 +8494,10 @@
     </row>
     <row r="126" ht="15.75" customHeight="1">
       <c r="A126" s="28" t="s">
-        <v>550</v>
+        <v>557</v>
       </c>
       <c r="B126" s="21" t="s">
-        <v>551</v>
+        <v>558</v>
       </c>
       <c r="C126" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8467,13 +8508,13 @@
         <v>optical_store_KGE24-0A-47</v>
       </c>
       <c r="E126" s="21" t="s">
-        <v>552</v>
+        <v>559</v>
       </c>
       <c r="F126" s="21" t="s">
-        <v>553</v>
+        <v>560</v>
       </c>
       <c r="G126" s="21" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="H126" s="4"/>
       <c r="I126" s="4"/>
@@ -8499,10 +8540,10 @@
     </row>
     <row r="127" ht="15.75" customHeight="1">
       <c r="A127" s="28" t="s">
-        <v>555</v>
+        <v>562</v>
       </c>
       <c r="B127" s="21" t="s">
-        <v>556</v>
+        <v>563</v>
       </c>
       <c r="C127" s="15" t="str">
         <f t="shared" si="9"/>
@@ -8513,13 +8554,13 @@
         <v>toy_store_KGE24-0A-48</v>
       </c>
       <c r="E127" s="21" t="s">
-        <v>557</v>
+        <v>564</v>
       </c>
       <c r="F127" s="21" t="s">
-        <v>558</v>
+        <v>565</v>
       </c>
       <c r="G127" s="21" t="s">
-        <v>554</v>
+        <v>561</v>
       </c>
       <c r="H127" s="4"/>
       <c r="I127" s="4"/>
@@ -8548,7 +8589,7 @@
       <c r="B128" s="67"/>
       <c r="C128" s="68"/>
       <c r="D128" s="68" t="s">
-        <v>559</v>
+        <v>566</v>
       </c>
       <c r="E128" s="7"/>
       <c r="F128" s="69"/>
@@ -8577,10 +8618,10 @@
     </row>
     <row r="129" ht="15.75" customHeight="1">
       <c r="A129" s="28" t="s">
-        <v>560</v>
+        <v>567</v>
       </c>
       <c r="B129" s="21" t="s">
-        <v>561</v>
+        <v>568</v>
       </c>
       <c r="C129" s="15" t="str">
         <f t="shared" ref="C129:C133" si="10">B129&amp;"_"&amp;A129</f>
@@ -8591,13 +8632,13 @@
         <v>sad_GID-81576</v>
       </c>
       <c r="E129" s="21" t="s">
-        <v>562</v>
+        <v>569</v>
       </c>
       <c r="F129" s="21" t="s">
-        <v>563</v>
+        <v>570</v>
       </c>
       <c r="G129" s="21" t="s">
-        <v>564</v>
+        <v>571</v>
       </c>
       <c r="H129" s="4"/>
       <c r="I129" s="4"/>
@@ -8623,10 +8664,10 @@
     </row>
     <row r="130" ht="15.75" customHeight="1">
       <c r="A130" s="28" t="s">
-        <v>565</v>
+        <v>572</v>
       </c>
       <c r="B130" s="21" t="s">
-        <v>566</v>
+        <v>573</v>
       </c>
       <c r="C130" s="15" t="str">
         <f t="shared" si="10"/>
@@ -8637,13 +8678,13 @@
         <v>down_GID-77954</v>
       </c>
       <c r="E130" s="21" t="s">
-        <v>567</v>
+        <v>574</v>
       </c>
       <c r="F130" s="21" t="s">
-        <v>568</v>
+        <v>575</v>
       </c>
       <c r="G130" s="21" t="s">
-        <v>569</v>
+        <v>576</v>
       </c>
       <c r="H130" s="4"/>
       <c r="I130" s="4"/>
@@ -8669,10 +8710,10 @@
     </row>
     <row r="131" ht="15.75" customHeight="1">
       <c r="A131" s="28" t="s">
-        <v>570</v>
+        <v>577</v>
       </c>
       <c r="B131" s="21" t="s">
-        <v>571</v>
+        <v>578</v>
       </c>
       <c r="C131" s="15" t="str">
         <f t="shared" si="10"/>
@@ -8683,13 +8724,13 @@
         <v>neutral_KGE24-0A-24</v>
       </c>
       <c r="E131" s="21" t="s">
-        <v>572</v>
+        <v>579</v>
       </c>
       <c r="F131" s="21" t="s">
-        <v>573</v>
+        <v>580</v>
       </c>
       <c r="G131" s="21" t="s">
-        <v>574</v>
+        <v>581</v>
       </c>
       <c r="H131" s="4"/>
       <c r="I131" s="4"/>
@@ -8715,10 +8756,10 @@
     </row>
     <row r="132" ht="15.75" customHeight="1">
       <c r="A132" s="28" t="s">
-        <v>575</v>
+        <v>582</v>
       </c>
       <c r="B132" s="21" t="s">
-        <v>576</v>
+        <v>583</v>
       </c>
       <c r="C132" s="15" t="str">
         <f t="shared" si="10"/>
@@ -8729,13 +8770,13 @@
         <v>happy_GID-80395</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>577</v>
+        <v>584</v>
       </c>
       <c r="F132" s="21" t="s">
-        <v>578</v>
+        <v>585</v>
       </c>
       <c r="G132" s="21" t="s">
-        <v>579</v>
+        <v>586</v>
       </c>
       <c r="H132" s="4"/>
       <c r="I132" s="4"/>
@@ -8761,10 +8802,10 @@
     </row>
     <row r="133" ht="15.75" customHeight="1">
       <c r="A133" s="28" t="s">
-        <v>580</v>
+        <v>587</v>
       </c>
       <c r="B133" s="21" t="s">
-        <v>581</v>
+        <v>588</v>
       </c>
       <c r="C133" s="15" t="str">
         <f t="shared" si="10"/>
@@ -8775,13 +8816,13 @@
         <v>excited_GID-79092</v>
       </c>
       <c r="E133" s="21" t="s">
-        <v>582</v>
+        <v>589</v>
       </c>
       <c r="F133" s="21" t="s">
-        <v>583</v>
+        <v>590</v>
       </c>
       <c r="G133" s="21" t="s">
-        <v>584</v>
+        <v>591</v>
       </c>
       <c r="H133" s="4"/>
       <c r="I133" s="4"/>
@@ -8810,7 +8851,7 @@
       <c r="B134" s="69"/>
       <c r="C134" s="68"/>
       <c r="D134" s="68" t="s">
-        <v>585</v>
+        <v>592</v>
       </c>
       <c r="E134" s="7"/>
       <c r="F134" s="69"/>
@@ -8839,10 +8880,10 @@
     </row>
     <row r="135" ht="15.75" customHeight="1">
       <c r="A135" s="28" t="s">
-        <v>586</v>
+        <v>593</v>
       </c>
       <c r="B135" s="21" t="s">
-        <v>587</v>
+        <v>594</v>
       </c>
       <c r="C135" s="15" t="str">
         <f t="shared" ref="C135:C164" si="12">B135&amp;"_"&amp;A135</f>
@@ -8853,13 +8894,13 @@
         <v>watching_GID-103268 </v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>588</v>
+        <v>595</v>
       </c>
       <c r="F135" s="21" t="s">
-        <v>589</v>
+        <v>596</v>
       </c>
       <c r="G135" s="21" t="s">
-        <v>590</v>
+        <v>597</v>
       </c>
       <c r="H135" s="4"/>
       <c r="I135" s="4"/>
@@ -8885,10 +8926,10 @@
     </row>
     <row r="136" ht="15.75" customHeight="1">
       <c r="A136" s="28" t="s">
-        <v>591</v>
+        <v>598</v>
       </c>
       <c r="B136" s="21" t="s">
-        <v>592</v>
+        <v>599</v>
       </c>
       <c r="C136" s="15" t="str">
         <f t="shared" si="12"/>
@@ -8899,13 +8940,13 @@
         <v>reading_GID-95695 </v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>593</v>
+        <v>600</v>
       </c>
       <c r="F136" s="21" t="s">
-        <v>594</v>
+        <v>601</v>
       </c>
       <c r="G136" s="21" t="s">
-        <v>595</v>
+        <v>602</v>
       </c>
       <c r="H136" s="4"/>
       <c r="I136" s="4"/>
@@ -8931,10 +8972,10 @@
     </row>
     <row r="137" ht="15.75" customHeight="1">
       <c r="A137" s="28" t="s">
-        <v>596</v>
+        <v>603</v>
       </c>
       <c r="B137" s="21" t="s">
-        <v>597</v>
+        <v>604</v>
       </c>
       <c r="C137" s="15" t="str">
         <f t="shared" si="12"/>
@@ -8945,13 +8986,13 @@
         <v>listening_to_GID-103365 </v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>598</v>
+        <v>605</v>
       </c>
       <c r="F137" s="21" t="s">
-        <v>599</v>
+        <v>606</v>
       </c>
       <c r="G137" s="21" t="s">
-        <v>600</v>
+        <v>607</v>
       </c>
       <c r="H137" s="4"/>
       <c r="I137" s="4"/>
@@ -8977,10 +9018,10 @@
     </row>
     <row r="138" ht="15.75" customHeight="1">
       <c r="A138" s="28" t="s">
-        <v>601</v>
+        <v>608</v>
       </c>
       <c r="B138" s="21" t="s">
-        <v>602</v>
+        <v>609</v>
       </c>
       <c r="C138" s="15" t="str">
         <f t="shared" si="12"/>
@@ -8991,13 +9032,13 @@
         <v>sleeping_GID-73617</v>
       </c>
       <c r="E138" s="21" t="s">
-        <v>603</v>
+        <v>610</v>
       </c>
       <c r="F138" s="21" t="s">
-        <v>604</v>
+        <v>611</v>
       </c>
       <c r="G138" s="21" t="s">
-        <v>605</v>
+        <v>612</v>
       </c>
       <c r="H138" s="4"/>
       <c r="I138" s="4"/>
@@ -9023,10 +9064,10 @@
     </row>
     <row r="139" ht="15.75" customHeight="1">
       <c r="A139" s="28" t="s">
-        <v>606</v>
+        <v>613</v>
       </c>
       <c r="B139" s="21" t="s">
-        <v>607</v>
+        <v>614</v>
       </c>
       <c r="C139" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9037,13 +9078,13 @@
         <v>studying_GID- 30956</v>
       </c>
       <c r="E139" s="21" t="s">
-        <v>608</v>
+        <v>615</v>
       </c>
       <c r="F139" s="21" t="s">
-        <v>609</v>
+        <v>616</v>
       </c>
       <c r="G139" s="21" t="s">
-        <v>610</v>
+        <v>617</v>
       </c>
       <c r="H139" s="4"/>
       <c r="I139" s="4"/>
@@ -9069,10 +9110,10 @@
     </row>
     <row r="140" ht="15.75" customHeight="1">
       <c r="A140" s="28" t="s">
-        <v>611</v>
+        <v>618</v>
       </c>
       <c r="B140" s="21" t="s">
-        <v>612</v>
+        <v>619</v>
       </c>
       <c r="C140" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9083,13 +9124,13 @@
         <v>eating_GID-4227</v>
       </c>
       <c r="E140" s="21" t="s">
-        <v>613</v>
+        <v>620</v>
       </c>
       <c r="F140" s="21" t="s">
-        <v>614</v>
+        <v>621</v>
       </c>
       <c r="G140" s="21" t="s">
-        <v>615</v>
+        <v>622</v>
       </c>
       <c r="H140" s="4"/>
       <c r="I140" s="4"/>
@@ -9115,10 +9156,10 @@
     </row>
     <row r="141" ht="15.75" customHeight="1">
       <c r="A141" s="28" t="s">
-        <v>616</v>
+        <v>623</v>
       </c>
       <c r="B141" s="21" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
       <c r="C141" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9129,13 +9170,13 @@
         <v>working_GID_2874</v>
       </c>
       <c r="E141" s="21" t="s">
-        <v>618</v>
+        <v>625</v>
       </c>
       <c r="F141" s="21" t="s">
-        <v>619</v>
+        <v>626</v>
       </c>
       <c r="G141" s="21" t="s">
-        <v>620</v>
+        <v>627</v>
       </c>
       <c r="H141" s="4"/>
       <c r="I141" s="4"/>
@@ -9161,10 +9202,10 @@
     </row>
     <row r="142" ht="15.75" customHeight="1">
       <c r="A142" s="28" t="s">
-        <v>621</v>
+        <v>628</v>
       </c>
       <c r="B142" s="21" t="s">
-        <v>622</v>
+        <v>629</v>
       </c>
       <c r="C142" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9175,10 +9216,10 @@
         <v>shopping_GID-303</v>
       </c>
       <c r="E142" s="21" t="s">
-        <v>623</v>
+        <v>630</v>
       </c>
       <c r="F142" s="21" t="s">
-        <v>624</v>
+        <v>631</v>
       </c>
       <c r="G142" s="73"/>
       <c r="H142" s="4"/>
@@ -9205,10 +9246,10 @@
     </row>
     <row r="143" ht="15.75" customHeight="1">
       <c r="A143" s="28" t="s">
-        <v>625</v>
+        <v>632</v>
       </c>
       <c r="B143" s="21" t="s">
-        <v>626</v>
+        <v>633</v>
       </c>
       <c r="C143" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9219,13 +9260,13 @@
         <v>pause_GID-5384</v>
       </c>
       <c r="E143" s="21" t="s">
-        <v>627</v>
+        <v>634</v>
       </c>
       <c r="F143" s="21" t="s">
-        <v>628</v>
+        <v>635</v>
       </c>
       <c r="G143" s="21" t="s">
-        <v>629</v>
+        <v>636</v>
       </c>
       <c r="H143" s="4"/>
       <c r="I143" s="4"/>
@@ -9251,10 +9292,10 @@
     </row>
     <row r="144" ht="15.75" customHeight="1">
       <c r="A144" s="28" t="s">
-        <v>630</v>
+        <v>637</v>
       </c>
       <c r="B144" s="21" t="s">
-        <v>631</v>
+        <v>638</v>
       </c>
       <c r="C144" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9265,13 +9306,13 @@
         <v>social_activity_GID-5475</v>
       </c>
       <c r="E144" s="21" t="s">
-        <v>632</v>
+        <v>639</v>
       </c>
       <c r="F144" s="21" t="s">
-        <v>633</v>
+        <v>640</v>
       </c>
       <c r="G144" s="21" t="s">
-        <v>634</v>
+        <v>641</v>
       </c>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -9297,10 +9338,10 @@
     </row>
     <row r="145" ht="15.75" customHeight="1">
       <c r="A145" s="28" t="s">
-        <v>635</v>
+        <v>642</v>
       </c>
       <c r="B145" s="21" t="s">
-        <v>636</v>
+        <v>643</v>
       </c>
       <c r="C145" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9311,13 +9352,13 @@
         <v>personal_care_KGE24-0A-21</v>
       </c>
       <c r="E145" s="21" t="s">
-        <v>637</v>
+        <v>644</v>
       </c>
       <c r="F145" s="21" t="s">
-        <v>638</v>
+        <v>645</v>
       </c>
       <c r="G145" s="21" t="s">
-        <v>639</v>
+        <v>646</v>
       </c>
       <c r="H145" s="4"/>
       <c r="I145" s="4"/>
@@ -9343,10 +9384,10 @@
     </row>
     <row r="146" ht="15.75" customHeight="1">
       <c r="A146" s="28" t="s">
-        <v>640</v>
+        <v>647</v>
       </c>
       <c r="B146" s="21" t="s">
-        <v>641</v>
+        <v>648</v>
       </c>
       <c r="C146" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9357,10 +9398,10 @@
         <v>hobby_GID- 2123</v>
       </c>
       <c r="E146" s="21" t="s">
-        <v>642</v>
+        <v>649</v>
       </c>
       <c r="F146" s="21" t="s">
-        <v>643</v>
+        <v>650</v>
       </c>
       <c r="G146" s="73"/>
       <c r="H146" s="4"/>
@@ -9387,10 +9428,10 @@
     </row>
     <row r="147" ht="15.75" customHeight="1">
       <c r="A147" s="28" t="s">
-        <v>644</v>
+        <v>651</v>
       </c>
       <c r="B147" s="21" t="s">
-        <v>645</v>
+        <v>652</v>
       </c>
       <c r="C147" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9401,13 +9442,13 @@
         <v>housework_KGE24-0A-22</v>
       </c>
       <c r="E147" s="21" t="s">
-        <v>646</v>
+        <v>653</v>
       </c>
       <c r="F147" s="21" t="s">
-        <v>647</v>
+        <v>654</v>
       </c>
       <c r="G147" s="21" t="s">
-        <v>648</v>
+        <v>655</v>
       </c>
       <c r="H147" s="4"/>
       <c r="I147" s="4"/>
@@ -9433,10 +9474,10 @@
     </row>
     <row r="148" ht="15.75" customHeight="1">
       <c r="A148" s="28" t="s">
-        <v>649</v>
+        <v>656</v>
       </c>
       <c r="B148" s="21" t="s">
-        <v>650</v>
+        <v>657</v>
       </c>
       <c r="C148" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9447,10 +9488,10 @@
         <v>coffee_break_GID-40097</v>
       </c>
       <c r="E148" s="21" t="s">
-        <v>651</v>
+        <v>658</v>
       </c>
       <c r="F148" s="21" t="s">
-        <v>652</v>
+        <v>659</v>
       </c>
       <c r="G148" s="73"/>
       <c r="H148" s="4"/>
@@ -9477,10 +9518,10 @@
     </row>
     <row r="149" ht="15.75" customHeight="1">
       <c r="A149" s="28" t="s">
-        <v>653</v>
+        <v>660</v>
       </c>
       <c r="B149" s="21" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="C149" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9491,13 +9532,13 @@
         <v>sport_GID-2593</v>
       </c>
       <c r="E149" s="21" t="s">
-        <v>655</v>
+        <v>662</v>
       </c>
       <c r="F149" s="21" t="s">
-        <v>654</v>
+        <v>661</v>
       </c>
       <c r="G149" s="21" t="s">
-        <v>656</v>
+        <v>663</v>
       </c>
       <c r="H149" s="4"/>
       <c r="I149" s="4"/>
@@ -9523,10 +9564,10 @@
     </row>
     <row r="150" ht="15.75" customHeight="1">
       <c r="A150" s="28" t="s">
-        <v>657</v>
+        <v>664</v>
       </c>
       <c r="B150" s="21" t="s">
-        <v>658</v>
+        <v>665</v>
       </c>
       <c r="C150" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9537,13 +9578,13 @@
         <v>other_KGE24-0A-23</v>
       </c>
       <c r="E150" s="74" t="s">
-        <v>659</v>
+        <v>666</v>
       </c>
       <c r="F150" s="21" t="s">
-        <v>660</v>
+        <v>667</v>
       </c>
       <c r="G150" s="21" t="s">
-        <v>661</v>
+        <v>668</v>
       </c>
       <c r="H150" s="4"/>
       <c r="I150" s="4"/>
@@ -9569,10 +9610,10 @@
     </row>
     <row r="151" ht="15.75" customHeight="1">
       <c r="A151" s="28" t="s">
-        <v>662</v>
+        <v>669</v>
       </c>
       <c r="B151" s="21" t="s">
-        <v>663</v>
+        <v>670</v>
       </c>
       <c r="C151" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9583,13 +9624,13 @@
         <v>lesson_GID-4491</v>
       </c>
       <c r="E151" s="74" t="s">
-        <v>664</v>
+        <v>671</v>
       </c>
       <c r="F151" s="21" t="s">
-        <v>665</v>
+        <v>672</v>
       </c>
       <c r="G151" s="21" t="s">
-        <v>666</v>
+        <v>673</v>
       </c>
       <c r="H151" s="4"/>
       <c r="I151" s="4"/>
@@ -9615,10 +9656,10 @@
     </row>
     <row r="152" ht="15.75" customHeight="1">
       <c r="A152" s="28" t="s">
-        <v>667</v>
+        <v>674</v>
       </c>
       <c r="B152" s="21" t="s">
-        <v>668</v>
+        <v>675</v>
       </c>
       <c r="C152" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9629,10 +9670,10 @@
         <v>movie_theater_GID-16033</v>
       </c>
       <c r="E152" s="74" t="s">
-        <v>669</v>
+        <v>676</v>
       </c>
       <c r="F152" s="21" t="s">
-        <v>670</v>
+        <v>677</v>
       </c>
       <c r="G152" s="73"/>
       <c r="H152" s="4"/>
@@ -9659,10 +9700,10 @@
     </row>
     <row r="153" ht="15.75" customHeight="1">
       <c r="A153" s="28" t="s">
-        <v>671</v>
+        <v>678</v>
       </c>
       <c r="B153" s="21" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
       <c r="C153" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9673,10 +9714,10 @@
         <v>social_media_KGE24-0A-25</v>
       </c>
       <c r="E153" s="74" t="s">
-        <v>673</v>
+        <v>680</v>
       </c>
       <c r="F153" s="21" t="s">
-        <v>672</v>
+        <v>679</v>
       </c>
       <c r="G153" s="73"/>
       <c r="H153" s="4"/>
@@ -9703,10 +9744,10 @@
     </row>
     <row r="154" ht="15.75" customHeight="1">
       <c r="A154" s="28" t="s">
-        <v>674</v>
+        <v>681</v>
       </c>
       <c r="B154" s="21" t="s">
-        <v>675</v>
+        <v>682</v>
       </c>
       <c r="C154" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9717,13 +9758,13 @@
         <v>en_route_GID-1415</v>
       </c>
       <c r="E154" s="74" t="s">
-        <v>676</v>
+        <v>683</v>
       </c>
       <c r="F154" s="21" t="s">
-        <v>677</v>
+        <v>684</v>
       </c>
       <c r="G154" s="21" t="s">
-        <v>678</v>
+        <v>685</v>
       </c>
       <c r="H154" s="4"/>
       <c r="I154" s="4"/>
@@ -9749,10 +9790,10 @@
     </row>
     <row r="155" ht="15.75" customHeight="1">
       <c r="A155" s="28" t="s">
-        <v>679</v>
+        <v>686</v>
       </c>
       <c r="B155" s="21" t="s">
-        <v>680</v>
+        <v>687</v>
       </c>
       <c r="C155" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9763,10 +9804,10 @@
         <v>on_the_phone_KGE24-0A-26</v>
       </c>
       <c r="E155" s="74" t="s">
-        <v>681</v>
+        <v>688</v>
       </c>
       <c r="F155" s="21" t="s">
-        <v>682</v>
+        <v>689</v>
       </c>
       <c r="G155" s="73"/>
       <c r="H155" s="4"/>
@@ -9793,10 +9834,10 @@
     </row>
     <row r="156" ht="15.75" customHeight="1">
       <c r="A156" s="28" t="s">
-        <v>683</v>
+        <v>690</v>
       </c>
       <c r="B156" s="21" t="s">
-        <v>684</v>
+        <v>691</v>
       </c>
       <c r="C156" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9807,10 +9848,10 @@
         <v>in_chat_KGE24-0A-27</v>
       </c>
       <c r="E156" s="74" t="s">
-        <v>685</v>
+        <v>692</v>
       </c>
       <c r="F156" s="21" t="s">
-        <v>686</v>
+        <v>693</v>
       </c>
       <c r="G156" s="73"/>
       <c r="H156" s="4"/>
@@ -9837,10 +9878,10 @@
     </row>
     <row r="157" ht="15.75" customHeight="1">
       <c r="A157" s="28" t="s">
-        <v>687</v>
+        <v>694</v>
       </c>
       <c r="B157" s="21" t="s">
-        <v>688</v>
+        <v>695</v>
       </c>
       <c r="C157" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9851,10 +9892,10 @@
         <v>free_time_GID-72882</v>
       </c>
       <c r="E157" s="74" t="s">
-        <v>689</v>
+        <v>696</v>
       </c>
       <c r="F157" s="21" t="s">
-        <v>690</v>
+        <v>697</v>
       </c>
       <c r="G157" s="73"/>
       <c r="H157" s="4"/>
@@ -9881,10 +9922,10 @@
     </row>
     <row r="158" ht="15.75" customHeight="1">
       <c r="A158" s="28" t="s">
-        <v>691</v>
+        <v>698</v>
       </c>
       <c r="B158" s="21" t="s">
-        <v>692</v>
+        <v>699</v>
       </c>
       <c r="C158" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9895,10 +9936,10 @@
         <v>cigarette_GID-4210</v>
       </c>
       <c r="E158" s="74" t="s">
-        <v>693</v>
+        <v>700</v>
       </c>
       <c r="F158" s="21" t="s">
-        <v>694</v>
+        <v>701</v>
       </c>
       <c r="G158" s="73"/>
       <c r="H158" s="4"/>
@@ -9925,10 +9966,10 @@
     </row>
     <row r="159" ht="15.75" customHeight="1">
       <c r="A159" s="28" t="s">
-        <v>695</v>
+        <v>702</v>
       </c>
       <c r="B159" s="21" t="s">
-        <v>696</v>
+        <v>703</v>
       </c>
       <c r="C159" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9939,10 +9980,10 @@
         <v>beer_GID-4255</v>
       </c>
       <c r="E159" s="74" t="s">
-        <v>697</v>
+        <v>704</v>
       </c>
       <c r="F159" s="21" t="s">
-        <v>698</v>
+        <v>705</v>
       </c>
       <c r="G159" s="73"/>
       <c r="H159" s="4"/>
@@ -9969,10 +10010,10 @@
     </row>
     <row r="160" ht="15.75" customHeight="1">
       <c r="A160" s="28" t="s">
-        <v>699</v>
+        <v>706</v>
       </c>
       <c r="B160" s="21" t="s">
-        <v>700</v>
+        <v>707</v>
       </c>
       <c r="C160" s="15" t="str">
         <f t="shared" si="12"/>
@@ -9983,10 +10024,10 @@
         <v>physical_activity_GID-3158</v>
       </c>
       <c r="E160" s="74" t="s">
-        <v>701</v>
+        <v>708</v>
       </c>
       <c r="F160" s="21" t="s">
-        <v>702</v>
+        <v>709</v>
       </c>
       <c r="G160" s="73"/>
       <c r="H160" s="4"/>
@@ -10013,10 +10054,10 @@
     </row>
     <row r="161" ht="15.75" customHeight="1">
       <c r="A161" s="28" t="s">
-        <v>703</v>
+        <v>710</v>
       </c>
       <c r="B161" s="75" t="s">
-        <v>704</v>
+        <v>711</v>
       </c>
       <c r="C161" s="15" t="str">
         <f t="shared" si="12"/>
@@ -10027,10 +10068,10 @@
         <v>rest_GID-5391</v>
       </c>
       <c r="E161" s="75" t="s">
-        <v>705</v>
+        <v>712</v>
       </c>
       <c r="F161" s="21" t="s">
-        <v>706</v>
+        <v>713</v>
       </c>
       <c r="G161" s="73"/>
       <c r="H161" s="4"/>
@@ -10057,10 +10098,10 @@
     </row>
     <row r="162" ht="15.75" customHeight="1">
       <c r="A162" s="28" t="s">
-        <v>707</v>
+        <v>714</v>
       </c>
       <c r="B162" s="75" t="s">
-        <v>708</v>
+        <v>715</v>
       </c>
       <c r="C162" s="15" t="str">
         <f t="shared" si="12"/>
@@ -10071,10 +10112,10 @@
         <v>nap_GID-4331</v>
       </c>
       <c r="E162" s="75" t="s">
-        <v>709</v>
+        <v>716</v>
       </c>
       <c r="F162" s="21" t="s">
-        <v>710</v>
+        <v>717</v>
       </c>
       <c r="G162" s="73"/>
       <c r="H162" s="4"/>
@@ -10101,10 +10142,10 @@
     </row>
     <row r="163" ht="15.75" customHeight="1">
       <c r="A163" s="28" t="s">
-        <v>711</v>
+        <v>718</v>
       </c>
       <c r="B163" s="75" t="s">
-        <v>712</v>
+        <v>719</v>
       </c>
       <c r="C163" s="15" t="str">
         <f t="shared" si="12"/>
@@ -10115,10 +10156,10 @@
         <v>fun_GID-2113</v>
       </c>
       <c r="E163" s="75" t="s">
-        <v>713</v>
+        <v>720</v>
       </c>
       <c r="F163" s="21" t="s">
-        <v>714</v>
+        <v>721</v>
       </c>
       <c r="G163" s="73"/>
       <c r="H163" s="4"/>
@@ -10145,10 +10186,10 @@
     </row>
     <row r="164" ht="15.75" customHeight="1">
       <c r="A164" s="28" t="s">
-        <v>715</v>
+        <v>722</v>
       </c>
       <c r="B164" s="75" t="s">
-        <v>716</v>
+        <v>723</v>
       </c>
       <c r="C164" s="15" t="str">
         <f t="shared" si="12"/>
@@ -10159,10 +10200,10 @@
         <v>exhibit_GID-4451</v>
       </c>
       <c r="E164" s="75" t="s">
-        <v>717</v>
+        <v>724</v>
       </c>
       <c r="F164" s="21" t="s">
-        <v>718</v>
+        <v>725</v>
       </c>
       <c r="G164" s="73"/>
       <c r="H164" s="4"/>

</xml_diff>